<commit_message>
Include the right model of the scenarios BAU and NDC
</commit_message>
<xml_diff>
--- a/t1_confection/A1_Outputs/A1_Outputs_BAU/A-O_AR_Model_Base_Year.xlsx
+++ b/t1_confection/A1_Outputs/A1_Outputs_BAU/A-O_AR_Model_Base_Year.xlsx
@@ -38813,8 +38813,8 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101000F48F53D8446FB4EB61FD3AFE2640F25" ma:contentTypeVersion="10" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="a214a3ba0c52ae00a3b9ea52e20da1dd">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7db9c71a-8f0f-4486-8c92-6242e053eab7" xmlns:ns3="8ae01698-3168-4e7f-b9e7-0ddc1c80de73" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1812e4edb338c892157ee4b16223776a" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000F48F53D8446FB4EB61FD3AFE2640F25" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c42e2caa13ae5d6057eea9be68815fce">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7db9c71a-8f0f-4486-8c92-6242e053eab7" xmlns:ns3="8ae01698-3168-4e7f-b9e7-0ddc1c80de73" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b95e89a8284191eba76f4506755f34ad" ns2:_="" ns3:_="">
     <xsd:import namespace="7db9c71a-8f0f-4486-8c92-6242e053eab7"/>
     <xsd:import namespace="8ae01698-3168-4e7f-b9e7-0ddc1c80de73"/>
     <xsd:element name="properties">
@@ -38857,7 +38857,7 @@
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="12" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Etiquetas de imagen" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="71f7bd95-1200-4052-9a4e-dfdf006e181b" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="12" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="71f7bd95-1200-4052-9a4e-dfdf006e181b" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
@@ -38911,8 +38911,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de contenido"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -39010,5 +39010,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{501EEC19-280C-42F3-B91D-A685C2B55EA6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2433209-4ECD-46AE-87E5-FA35C7745A39}"/>
 </file>
</xml_diff>